<commit_message>
Alcatel AOS devices in test
</commit_message>
<xml_diff>
--- a/test_plan.xlsx
+++ b/test_plan.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="21">
   <si>
     <t>Cisco IOS</t>
   </si>
@@ -465,7 +465,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -498,8 +498,8 @@
       <c r="C2" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>20</v>
+      <c r="D2" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>20</v>
@@ -526,7 +526,9 @@
         <v>6</v>
       </c>
       <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
+      <c r="D4" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="E4" s="3"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -545,8 +547,8 @@
       <c r="C6" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="7" t="s">
-        <v>20</v>
+      <c r="D6" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>20</v>
@@ -573,7 +575,9 @@
         <v>6</v>
       </c>
       <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
+      <c r="D8" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="E8" s="3"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -584,7 +588,9 @@
         <v>6</v>
       </c>
       <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
+      <c r="D9" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="E9" s="3"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -603,8 +609,8 @@
       <c r="C11" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="7" t="s">
-        <v>20</v>
+      <c r="D11" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>20</v>
@@ -683,7 +689,9 @@
         <v>6</v>
       </c>
       <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
+      <c r="D17" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="E17" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Telnet and SSH tested on 3 devices
</commit_message>
<xml_diff>
--- a/test_plan.xlsx
+++ b/test_plan.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="22">
   <si>
     <t xml:space="preserve">Cisco S300</t>
   </si>
@@ -309,13 +309,13 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2:C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.02"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -332,15 +332,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>6</v>
+      <c r="C2" s="3" t="s">
+        <v>5</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>5</v>
@@ -349,7 +349,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
         <v>7</v>
       </c>
@@ -364,14 +364,16 @@
       </c>
       <c r="E3" s="6"/>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="6"/>
+      <c r="C4" s="6" t="s">
+        <v>8</v>
+      </c>
       <c r="D4" s="6" t="s">
         <v>8</v>
       </c>

</xml_diff>